<commit_message>
PQ Challenge 5 and 6 is solved using lambda.
</commit_message>
<xml_diff>
--- a/Excel Files/PQ Challenges/PQ Challenge 4 Problem.xlsx
+++ b/Excel Files/PQ Challenges/PQ Challenge 4 Problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\PQ Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF447F96-2CD4-462C-9596-4CF09529D3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C935D9B-D330-4F5C-AF7F-051D59DD1B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{96679C68-C62D-4D07-97DF-11B9EB0C2887}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <definedName name="UNPIVOT">_xlfn.LAMBDA(_xlpm.table,_xlpm.columns_to_unpivot,_xlop.attribute_name,_xlop.value_name,_xlop.remove_blanks, _xlfn.LET(_xlpm.AttributeLabel, IF(_xlfn.ISOMITTED(_xlpm.attribute_name), "Attribute", _xlpm.attribute_name), _xlpm.ValueLabel, IF(_xlfn.ISOMITTED(_xlpm.value_name), "Value", _xlpm.value_name), _xlpm.FirstColumnToUnpivot, MATCH(INDEX(_xlpm.columns_to_unpivot, , 1), INDEX(_xlpm.table, 1, ), 0), _xlpm.UnpivotColumnCount, COLUMNS(_xlpm.columns_to_unpivot), _xlpm.ColumnNumbers, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.table)), _xlpm.UnpivotColumns, _xlfn._xlws.FILTER(_xlpm.ColumnNumbers, (_xlpm.ColumnNumbers &gt;= _xlpm.FirstColumnToUnpivot) * (_xlpm.ColumnNumbers &lt; _xlpm.FirstColumnToUnpivot + _xlpm.UnpivotColumnCount)), _xlpm.OtherColumns, _xlfn._xlws.FILTER(_xlpm.ColumnNumbers, (_xlpm.ColumnNumbers &lt; _xlpm.FirstColumnToUnpivot) + (_xlpm.ColumnNumbers &gt;= _xlpm.FirstColumnToUnpivot + _xlpm.UnpivotColumnCount)), _xlpm.FullOuterJoin, CROSSJOIN(_xlfn.CHOOSECOLS(_xlpm.table, _xlpm.OtherColumns), _xlfn.VSTACK(_xlpm.AttributeLabel, TRANSPOSE(_xlpm.columns_to_unpivot))), _xlpm.WithValues, _xlfn.HSTACK(_xlpm.FullOuterJoin, _xlfn.VSTACK(_xlpm.ValueLabel, _xlfn.TOCOL(_xlfn.DROP(_xlfn.CHOOSECOLS(_xlpm.table, _xlpm.UnpivotColumns), 1)))), _xlpm.RemoveBlanks, IF(OR(_xlfn.ISOMITTED(_xlpm.remove_blanks), _xlpm.remove_blanks), _xlfn._xlws.FILTER(_xlpm.WithValues, INDEX(_xlpm.WithValues, , COLUMNS(_xlpm.WithValues)) &lt;&gt; ""), IF(_xlpm.WithValues = "", "", _xlpm.WithValues)), _xlpm.ColumnOrder, _xlfn.LET(_xlpm.n, COLUMNS(_xlpm.RemoveBlanks), _xlpm.s, _xlfn.SEQUENCE(1, _xlpm.n), _xlfn.IFS(_xlpm.s &lt; _xlpm.FirstColumnToUnpivot, _xlpm.s, _xlpm.s &lt; _xlpm.FirstColumnToUnpivot + 2, _xlpm.s + _xlpm.n - _xlpm.FirstColumnToUnpivot - 1, TRUE, _xlpm.s - 2)), _xlpm.ReorderColumns, _xlfn.CHOOSECOLS(_xlpm.RemoveBlanks, _xlpm.ColumnOrder), _xlpm.ReorderColumns))</definedName>
     <definedName name="ValueMatcher">_xlfn.LAMBDA(_xlpm.Vector,_xlpm.Operator,_xlpm.MatchValue, _xlfn.SWITCH(_xlpm.Operator, "=", _xlpm.Vector = _xlpm.MatchValue, "&lt;&gt;", _xlpm.Vector &lt;&gt; _xlpm.MatchValue, "&gt;", _xlpm.Vector &gt; _xlpm.MatchValue, "&lt;", _xlpm.Vector &lt; _xlpm.MatchValue, "&gt;=", _xlpm.Vector &gt;= _xlpm.MatchValue, "&lt;=", _xlpm.Vector &lt;= _xlpm.MatchValue, NA()))</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,6 +70,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -190,9 +191,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="dd\ mmm\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="164" formatCode="dd\ mmm\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -357,12 +358,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,6 +1356,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1370,7 +1374,7 @@
   <dimension ref="B1:U17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1426,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="P2" t="str" cm="1">
-        <f t="array" ref="P2:U10">_xlfn.LET(_xlpm.SalesData, B3:E15, _xlpm.fx_OneRowCleanUp, _xlfn.LAMBDA(_xlpm.OneRowData, _xlfn.LET(_xlpm.OneRowData2, B3:E3, _xlpm.Name, TRIM(SUBSTITUTE(INDEX(_xlpm.OneRowData, 1, 2), " ", "")), _xlpm.SplittedName, _xlfn.TEXTSPLIT(_xlpm.Name, , "/"), _xlpm.OrderNumber, INDEX(_xlpm.OneRowData, 1, 1), _xlpm.Date, INDEX(_xlpm.OneRowData, 1, 3), _xlpm.Amount, INDEX(_xlpm.OneRowData, 1, 4) / ROWS(_xlpm.SplittedName), _xlpm.Result, BYROWVSTACKER(_xlpm.SplittedName, _xlfn.LAMBDA(_xlpm.Curr, _xlfn.HSTACK(_xlpm.OrderNumber, _xlpm.Curr, _xlpm.Date, _xlpm.Amount))), _xlpm.Result)), _xlpm.CleanData, BYROWVSTACKER(_xlpm.SalesData, _xlpm.fx_OneRowCleanUp), _xlpm.DateData, _xlfn.CHOOSECOLS(_xlpm.CleanData, 3), _xlpm.MonthNames, TEXT(_xlpm.DateData, "mmm"), _xlpm.UniqueMonthNames, TRANSPOSE(_xlfn.UNIQUE(TEXT(_xlfn._xlws.SORT(_xlpm.DateData), "mmm"))), _xlpm.UniqueName, _xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.CleanData, 2))), _xlpm.OrderDataWithMonthName, _xlfn.HSTACK(_xlpm.CleanData, _xlpm.MonthNames), _xlpm.Header, _xlfn.HSTACK("Name", "Order Nos.", _xlpm.UniqueMonthNames, "Total"), _xlpm.fx_ForOneName, _xlfn.LAMBDA(_xlpm.Data,_xlpm.Name, _xlfn.LET(_xlpm.FilteredData, _xlfn._xlws.FILTER(_xlpm.Data, _xlfn.CHOOSECOLS(_xlpm.Data, 2) = _xlpm.Name), _xlpm.OrdersNo, _xlfn.TEXTJOIN(",", FALSE, _xlfn.CHOOSECOLS(_xlpm.FilteredData, 1)), _xlpm.MonthWiseSum, _xlfn.MAP(_xlpm.UniqueMonthNames, _xlfn.LAMBDA(_xlpm.Curr, IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.FilteredData, 4), _xlfn.CHOOSECOLS(_xlpm.FilteredData, 5) = _xlpm.Curr)), ""))), _xlpm.Total, SUM(_xlfn.CHOOSECOLS(_xlpm.FilteredData, 4)), _xlpm.Result, _xlfn.HSTACK(_xlpm.Name, _xlpm.OrdersNo, _xlpm.MonthWiseSum, _xlpm.Total), _xlpm.Result2, _xlfn.VSTACK(_xlpm.Header, _xlpm.Result), _xlpm.Result)), _xlpm.OneNameEx, _xlpm.fx_ForOneName(_xlpm.OrderDataWithMonthName, "Bob"), _xlpm.AllNames, BYROWVSTACKER(_xlpm.UniqueName, _xlfn.LAMBDA(_xlpm.Curr, _xlpm.fx_ForOneName(_xlpm.OrderDataWithMonthName, _xlpm.Curr))), _xlpm.Result, _xlfn.VSTACK(_xlpm.Header, _xlpm.AllNames), _xlpm.Result)</f>
+        <f t="array" ref="P2:U10">_xlfn.LAMBDA(_xlpm.SalesData, _xlfn.LET(_xlpm.SalesData2, B3:E15, _xlpm.fx_OneRowCleanUp, _xlfn.LAMBDA(_xlpm.OneRowData, _xlfn.LET(_xlpm.OneRowData2, {1001,"John",44362,11.91}, _xlpm.Name, TRIM(SUBSTITUTE(INDEX(_xlpm.OneRowData, 1, 2), " ", "")), _xlpm.SplittedName, _xlfn.TEXTSPLIT(_xlpm.Name, , "/"), _xlpm.OrderNumber, INDEX(_xlpm.OneRowData, 1, 1), _xlpm.Date, INDEX(_xlpm.OneRowData, 1, 3), _xlpm.Amount, INDEX(_xlpm.OneRowData, 1, 4) / ROWS(_xlpm.SplittedName), _xlpm.Result, BYROWVSTACKER(_xlpm.SplittedName, _xlfn.LAMBDA(_xlpm.Curr, _xlfn.HSTACK(_xlpm.OrderNumber, _xlpm.Curr, _xlpm.Date, _xlpm.Amount))), _xlpm.Result)), _xlpm.CleanData, BYROWVSTACKER(_xlpm.SalesData, _xlpm.fx_OneRowCleanUp), _xlpm.DateData, _xlfn.CHOOSECOLS(_xlpm.CleanData, 3), _xlpm.MonthNames, TEXT(_xlpm.DateData, "mmm"), _xlpm.UniqueMonthNames, TRANSPOSE(_xlfn.UNIQUE(TEXT(_xlfn._xlws.SORT(_xlpm.DateData), "mmm"))), _xlpm.UniqueName, _xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.CleanData, 2))), _xlpm.OrderDataWithMonthName, _xlfn.HSTACK(_xlpm.CleanData, _xlpm.MonthNames), _xlpm.Header, _xlfn.HSTACK("Name", "Order Nos.", _xlpm.UniqueMonthNames, "Total"), _xlpm.fx_ForOneName, _xlfn.LAMBDA(_xlpm.Data,_xlpm.Name, _xlfn.LET(_xlpm.FilteredData, _xlfn._xlws.FILTER(_xlpm.Data, _xlfn.CHOOSECOLS(_xlpm.Data, 2) = _xlpm.Name), _xlpm.OrdersNo, _xlfn.TEXTJOIN(",", FALSE, _xlfn.CHOOSECOLS(_xlpm.FilteredData, 1)), _xlpm.MonthWiseSum, _xlfn.MAP(_xlpm.UniqueMonthNames, _xlfn.LAMBDA(_xlpm.Curr, IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.FilteredData, 4), _xlfn.CHOOSECOLS(_xlpm.FilteredData, 5) = _xlpm.Curr)), ""))), _xlpm.Total, SUM(_xlfn.CHOOSECOLS(_xlpm.FilteredData, 4)), _xlpm.Result, _xlfn.HSTACK(_xlpm.Name, _xlpm.OrdersNo, _xlpm.MonthWiseSum, _xlpm.Total), _xlpm.Result2, _xlfn.VSTACK(_xlpm.Header, _xlpm.Result), _xlpm.Result)), _xlpm.OneNameEx, _xlpm.fx_ForOneName(_xlpm.OrderDataWithMonthName, "Bob"), _xlpm.AllNames, BYROWVSTACKER(_xlpm.UniqueName, _xlfn.LAMBDA(_xlpm.Curr, _xlpm.fx_ForOneName(_xlpm.OrderDataWithMonthName, _xlpm.Curr))), _xlpm.Result, _xlfn.VSTACK(_xlpm.Header, _xlpm.AllNames), _xlpm.Result))(B3:E15)</f>
         <v>Name</v>
       </c>
       <c r="Q2" t="str">

</xml_diff>